<commit_message>
Started testing my Horus cards, and adjusting the results spreadsheet as I realise I need different functionality from it.
</commit_message>
<xml_diff>
--- a/Custom Cards/Horus the Black Flame Dragon/Playtest Results.xlsx
+++ b/Custom Cards/Horus the Black Flame Dragon/Playtest Results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samhu\Documents\Documents\Game Design\Custom Yu-Gi-Oh! Cards\Custom Archetype Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samhu\Documents\Documents\Game Design\Custom Yu-Gi-Oh! Cards\Custom Cards\Horus the Black Flame Dragon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B9E352BB-BA07-4996-A2A9-3B87339F350D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB2A1D55-9B73-466B-B42F-5CE9085EF75B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{AD9CF55C-5A2C-43F9-8449-28DA4DBE7F5E}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="4" xr2:uid="{AD9CF55C-5A2C-43F9-8449-28DA4DBE7F5E}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Environment Changes" sheetId="6" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="73">
   <si>
     <t>Deck</t>
   </si>
@@ -201,6 +201,54 @@
   </si>
   <si>
     <t>Must sort A:C by Date, Newest to Oldest for formula to work correctly</t>
+  </si>
+  <si>
+    <t>Match Win %</t>
+  </si>
+  <si>
+    <t>Duel Win %</t>
+  </si>
+  <si>
+    <t>Chaos Turbo</t>
+  </si>
+  <si>
+    <t>Chaos Warriors</t>
+  </si>
+  <si>
+    <t>Warriors</t>
+  </si>
+  <si>
+    <t>Empty Jar</t>
+  </si>
+  <si>
+    <t>Library FTK</t>
+  </si>
+  <si>
+    <t>Reasoning Gate</t>
+  </si>
+  <si>
+    <t>Rescue Cat</t>
+  </si>
+  <si>
+    <t>Chaos Return</t>
+  </si>
+  <si>
+    <t>Goat Control</t>
+  </si>
+  <si>
+    <t>Recruiter Chaos</t>
+  </si>
+  <si>
+    <t>Chaos Control (Angel)</t>
+  </si>
+  <si>
+    <t>Chaos Control (Thunder Dragon)</t>
+  </si>
+  <si>
+    <t>Chaos Control (Skilled White Magician)</t>
+  </si>
+  <si>
+    <t>Win</t>
   </si>
 </sst>
 </file>
@@ -208,10 +256,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="mmm\-yyyy"/>
-    <numFmt numFmtId="166" formatCode="d/mm/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="mmm\-yyyy"/>
+    <numFmt numFmtId="165" formatCode="d/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -221,6 +269,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -245,16 +300,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -267,12 +323,23 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -651,7 +718,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
-      <c r="F4" s="12"/>
+      <c r="F4"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
@@ -751,10 +818,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DC8C623-D4B8-4C22-A988-D9BD9517564D}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -788,251 +855,251 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
-        <f>INDEX(Formats!A:A, MATCH(B2, Formats!B:B, 0), 0)</f>
-        <v>40269</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>23</v>
+        <v>38565</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="12">
+        <v>1</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>59</v>
       </c>
       <c r="E2" t="s">
         <v>36</v>
       </c>
+      <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
-        <f>INDEX(Formats!A:A, MATCH(B3, Formats!B:B, 0), 0)</f>
-        <v>40269</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>24</v>
+        <v>38565</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="12">
+        <v>1</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>60</v>
       </c>
       <c r="E3" t="s">
         <v>36</v>
       </c>
+      <c r="F3" s="12"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
-        <f>INDEX(Formats!A:A, MATCH(B4, Formats!B:B, 0), 0)</f>
-        <v>40269</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>25</v>
+        <v>38565</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="12">
+        <v>1</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>61</v>
       </c>
       <c r="E4" t="s">
         <v>36</v>
       </c>
+      <c r="F4" s="12"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
-        <f>INDEX(Formats!A:A, MATCH(B5, Formats!B:B, 0), 0)</f>
-        <v>40269</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-      <c r="D5" t="s">
-        <v>26</v>
+        <v>38565</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="12">
+        <v>2</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>69</v>
       </c>
       <c r="E5" t="s">
         <v>36</v>
       </c>
+      <c r="F5" s="12"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
-        <f>INDEX(Formats!A:A, MATCH(B6, Formats!B:B, 0), 0)</f>
-        <v>40269</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
-      <c r="D6" t="s">
-        <v>27</v>
+        <v>38565</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="12">
+        <v>2</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>70</v>
       </c>
       <c r="E6" t="s">
         <v>36</v>
       </c>
+      <c r="F6" s="12"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
-        <f>INDEX(Formats!A:A, MATCH(B7, Formats!B:B, 0), 0)</f>
-        <v>41821</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>5</v>
+        <v>38565</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="12">
+        <v>2</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>71</v>
       </c>
       <c r="E7" t="s">
         <v>36</v>
       </c>
+      <c r="F7" s="12"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
-        <f>INDEX(Formats!A:A, MATCH(B8, Formats!B:B, 0), 0)</f>
-        <v>41821</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>4</v>
+        <v>38565</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="12">
+        <v>2</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="E8" t="s">
         <v>36</v>
       </c>
+      <c r="F8" s="12"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
-        <f>INDEX(Formats!A:A, MATCH(B9, Formats!B:B, 0), 0)</f>
-        <v>41821</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>2</v>
+        <v>38565</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="12">
+        <v>2</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>62</v>
       </c>
       <c r="E9" t="s">
         <v>36</v>
       </c>
+      <c r="F9" s="12"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
-        <f>INDEX(Formats!A:A, MATCH(B10, Formats!B:B, 0), 0)</f>
-        <v>41821</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>6</v>
+        <v>38565</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="12">
+        <v>2</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>67</v>
       </c>
       <c r="E10" t="s">
         <v>36</v>
       </c>
+      <c r="F10" s="12"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
-        <f>INDEX(Formats!A:A, MATCH(B11, Formats!B:B, 0), 0)</f>
-        <v>41821</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>7</v>
+        <v>38565</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="12">
+        <v>2</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>63</v>
       </c>
       <c r="E11" t="s">
         <v>36</v>
       </c>
+      <c r="F11" s="12"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
-        <f>INDEX(Formats!A:A, MATCH(B12, Formats!B:B, 0), 0)</f>
-        <v>41821</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
-      <c r="D12" t="s">
-        <v>8</v>
+        <v>38565</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="12">
+        <v>2</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>64</v>
       </c>
       <c r="E12" t="s">
         <v>36</v>
       </c>
+      <c r="F12" s="12"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
-        <f>INDEX(Formats!A:A, MATCH(B13, Formats!B:B, 0), 0)</f>
-        <v>41821</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13">
-        <v>2</v>
-      </c>
-      <c r="D13" t="s">
-        <v>9</v>
+        <v>38565</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="12">
+        <v>2</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>68</v>
       </c>
       <c r="E13" t="s">
         <v>36</v>
       </c>
+      <c r="F13" s="12"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
-        <f>INDEX(Formats!A:A, MATCH(B14, Formats!B:B, 0), 0)</f>
-        <v>41821</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14">
-        <v>2</v>
-      </c>
-      <c r="D14" t="s">
-        <v>10</v>
+        <v>38565</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="12">
+        <v>2</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="E14" t="s">
         <v>36</v>
       </c>
+      <c r="F14" s="12"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <f>INDEX(Formats!A:A, MATCH(B15, Formats!B:B, 0), 0)</f>
-        <v>41821</v>
+        <v>40269</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="C15">
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="E15" t="s">
         <v>36</v>
@@ -1041,16 +1108,16 @@
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <f>INDEX(Formats!A:A, MATCH(B16, Formats!B:B, 0), 0)</f>
-        <v>41821</v>
+        <v>40269</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="C16">
         <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E16" t="s">
         <v>36</v>
@@ -1059,16 +1126,16 @@
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <f>INDEX(Formats!A:A, MATCH(B17, Formats!B:B, 0), 0)</f>
-        <v>41821</v>
+        <v>40269</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="C17">
         <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="E17" t="s">
         <v>36</v>
@@ -1077,16 +1144,16 @@
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <f>INDEX(Formats!A:A, MATCH(B18, Formats!B:B, 0), 0)</f>
-        <v>41821</v>
+        <v>40269</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="C18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D18" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="E18" t="s">
         <v>36</v>
@@ -1095,16 +1162,16 @@
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <f>INDEX(Formats!A:A, MATCH(B19, Formats!B:B, 0), 0)</f>
-        <v>41821</v>
+        <v>40269</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="C19">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D19" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="E19" t="s">
         <v>36</v>
@@ -1119,10 +1186,10 @@
         <v>2</v>
       </c>
       <c r="C20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="E20" t="s">
         <v>36</v>
@@ -1137,10 +1204,10 @@
         <v>2</v>
       </c>
       <c r="C21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="E21" t="s">
         <v>36</v>
@@ -1155,10 +1222,10 @@
         <v>2</v>
       </c>
       <c r="C22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="E22" t="s">
         <v>36</v>
@@ -1173,10 +1240,10 @@
         <v>2</v>
       </c>
       <c r="C23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="E23" t="s">
         <v>36</v>
@@ -1191,10 +1258,10 @@
         <v>2</v>
       </c>
       <c r="C24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="E24" t="s">
         <v>36</v>
@@ -1208,22 +1275,256 @@
       <c r="B25" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
       <c r="D25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <f>INDEX(Formats!A:A, MATCH(B26, Formats!B:B, 0), 0)</f>
+        <v>41821</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <f>INDEX(Formats!A:A, MATCH(B27, Formats!B:B, 0), 0)</f>
+        <v>41821</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <f>INDEX(Formats!A:A, MATCH(B28, Formats!B:B, 0), 0)</f>
+        <v>41821</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <f>INDEX(Formats!A:A, MATCH(B29, Formats!B:B, 0), 0)</f>
+        <v>41821</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <f>INDEX(Formats!A:A, MATCH(B30, Formats!B:B, 0), 0)</f>
+        <v>41821</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="D30" t="s">
+        <v>13</v>
+      </c>
+      <c r="E30" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <f>INDEX(Formats!A:A, MATCH(B31, Formats!B:B, 0), 0)</f>
+        <v>41821</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31" t="s">
+        <v>14</v>
+      </c>
+      <c r="E31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
+        <f>INDEX(Formats!A:A, MATCH(B32, Formats!B:B, 0), 0)</f>
+        <v>41821</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="D32" t="s">
+        <v>15</v>
+      </c>
+      <c r="E32" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
+        <f>INDEX(Formats!A:A, MATCH(B33, Formats!B:B, 0), 0)</f>
+        <v>41821</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="D33" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
+        <f>INDEX(Formats!A:A, MATCH(B34, Formats!B:B, 0), 0)</f>
+        <v>41821</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="D34" t="s">
+        <v>16</v>
+      </c>
+      <c r="E34" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
+        <f>INDEX(Formats!A:A, MATCH(B35, Formats!B:B, 0), 0)</f>
+        <v>41821</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
+      </c>
+      <c r="D35" t="s">
+        <v>18</v>
+      </c>
+      <c r="E35" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <f>INDEX(Formats!A:A, MATCH(B36, Formats!B:B, 0), 0)</f>
+        <v>41821</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36">
+        <v>2</v>
+      </c>
+      <c r="D36" t="s">
+        <v>19</v>
+      </c>
+      <c r="E36" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
+        <f>INDEX(Formats!A:A, MATCH(B37, Formats!B:B, 0), 0)</f>
+        <v>41821</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
+      <c r="D37" t="s">
+        <v>20</v>
+      </c>
+      <c r="E37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="4">
+        <f>INDEX(Formats!A:A, MATCH(B38, Formats!B:B, 0), 0)</f>
+        <v>41821</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D38" t="s">
         <v>37</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E38" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="2"/>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B39" s="2"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F26">
-    <sortCondition ref="A2:A26"/>
-    <sortCondition descending="1" ref="E2:E26"/>
-    <sortCondition ref="C2:C26"/>
-    <sortCondition ref="D2:D26"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F40">
+    <sortCondition ref="A2:A40"/>
+    <sortCondition descending="1" ref="E2:E40"/>
+    <sortCondition ref="C2:C40"/>
+    <sortCondition ref="D2:D40"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1231,14 +1532,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41E830D7-F746-4F8D-8170-0D055311D58C}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:H5"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
@@ -1271,64 +1573,108 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="2">
-        <f>INDEX(Formats!A:A, MATCH(C2, Formats!B:B, 0), 0)</f>
-        <v>40269</v>
-      </c>
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" t="s">
-        <v>23</v>
+      <c r="A2" s="9">
+        <v>45608</v>
+      </c>
+      <c r="B2" s="4">
+        <v>38565</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="2">
-        <f>INDEX(Formats!A:A, MATCH(C3, Formats!B:B, 0), 0)</f>
-        <v>41821</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="2">
-        <f>INDEX(Formats!A:A, MATCH(C4, Formats!B:B, 0), 0)</f>
-        <v>40269</v>
-      </c>
-      <c r="C4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" t="s">
-        <v>24</v>
-      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="2">
-        <f>INDEX(Formats!A:A, MATCH(C5, Formats!B:B, 0), 0)</f>
-        <v>40269</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
-      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="4"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="4"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="4"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="4"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="4"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="4"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="2"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H16">
+    <sortCondition ref="B2:B16"/>
+    <sortCondition ref="D2:D16"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{226CDD82-E2CC-4FA6-A945-41CFC8AD47C7}">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:K25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1341,12 +1687,14 @@
     <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.42578125" style="14" customWidth="1"/>
+    <col min="10" max="10" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.140625" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="8" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="8" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>34</v>
       </c>
@@ -1371,36 +1719,41 @@
       <c r="H1" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M1" s="15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
-        <f>INDEX(Formats!A:A, MATCH(B2, Formats!B:B, 0), 0)</f>
-        <v>40269</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>23</v>
+        <v>38565</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="12">
+        <v>1</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>59</v>
       </c>
       <c r="E2" t="s">
         <v>36</v>
       </c>
       <c r="F2">
         <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A2, 'Match Records'!D:D, 'Match Records Overview'!D2, 'Match Records'!H:H, "Win")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2">
         <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A2, 'Match Records'!D:D, 'Match Records Overview'!D2, 'Match Records'!H:H, "Lose")</f>
@@ -1410,32 +1763,39 @@
         <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A2, 'Match Records'!D:D, 'Match Records Overview'!D2, 'Match Records'!H:H, "Draw")</f>
         <v>0</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="14">
+        <f>F2/SUM(F2:G2)</f>
+        <v>1</v>
+      </c>
+      <c r="J2">
         <f>SUMIFS('Match Records'!E:E, 'Match Records'!B:B, 'Match Records Overview'!A2, 'Match Records'!D:D, 'Match Records Overview'!D2)</f>
-        <v>0</v>
-      </c>
-      <c r="J2">
+        <v>2</v>
+      </c>
+      <c r="K2">
         <f>SUMIFS('Match Records'!F:F, 'Match Records'!B:B, 'Match Records Overview'!A2, 'Match Records'!D:D, 'Match Records Overview'!D2)</f>
         <v>0</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <f>SUMIFS('Match Records'!G:G, 'Match Records'!B:B, 'Match Records Overview'!A2, 'Match Records'!D:D, 'Match Records Overview'!D2)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M2" s="16">
+        <f>J2/SUM(J2:K2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
-        <f>INDEX(Formats!A:A, MATCH(B3, Formats!B:B, 0), 0)</f>
-        <v>40269</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>24</v>
+        <v>38565</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="12">
+        <v>1</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>60</v>
       </c>
       <c r="E3" t="s">
         <v>36</v>
@@ -1452,32 +1812,39 @@
         <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A3, 'Match Records'!D:D, 'Match Records Overview'!D3, 'Match Records'!H:H, "Draw")</f>
         <v>0</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="14" t="e">
+        <f t="shared" ref="I3:I36" si="0">F3/SUM(F3:G3)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J3">
         <f>SUMIFS('Match Records'!E:E, 'Match Records'!B:B, 'Match Records Overview'!A3, 'Match Records'!D:D, 'Match Records Overview'!D3)</f>
         <v>0</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <f>SUMIFS('Match Records'!F:F, 'Match Records'!B:B, 'Match Records Overview'!A3, 'Match Records'!D:D, 'Match Records Overview'!D3)</f>
         <v>0</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <f>SUMIFS('Match Records'!G:G, 'Match Records'!B:B, 'Match Records Overview'!A3, 'Match Records'!D:D, 'Match Records Overview'!D3)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M3" s="16" t="e">
+        <f t="shared" ref="M3:M36" si="1">J3/SUM(J3:K3)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
-        <f>INDEX(Formats!A:A, MATCH(B4, Formats!B:B, 0), 0)</f>
-        <v>40269</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>25</v>
+        <v>38565</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="12">
+        <v>1</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>61</v>
       </c>
       <c r="E4" t="s">
         <v>36</v>
@@ -1494,32 +1861,39 @@
         <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A4, 'Match Records'!D:D, 'Match Records Overview'!D4, 'Match Records'!H:H, "Draw")</f>
         <v>0</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="14" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J4">
         <f>SUMIFS('Match Records'!E:E, 'Match Records'!B:B, 'Match Records Overview'!A4, 'Match Records'!D:D, 'Match Records Overview'!D4)</f>
         <v>0</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <f>SUMIFS('Match Records'!F:F, 'Match Records'!B:B, 'Match Records Overview'!A4, 'Match Records'!D:D, 'Match Records Overview'!D4)</f>
         <v>0</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <f>SUMIFS('Match Records'!G:G, 'Match Records'!B:B, 'Match Records Overview'!A4, 'Match Records'!D:D, 'Match Records Overview'!D4)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M4" s="16" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
-        <f>INDEX(Formats!A:A, MATCH(B5, Formats!B:B, 0), 0)</f>
-        <v>40269</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-      <c r="D5" t="s">
-        <v>26</v>
+        <v>38565</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="12">
+        <v>2</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>69</v>
       </c>
       <c r="E5" t="s">
         <v>36</v>
@@ -1536,32 +1910,39 @@
         <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A5, 'Match Records'!D:D, 'Match Records Overview'!D5, 'Match Records'!H:H, "Draw")</f>
         <v>0</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="14" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J5">
         <f>SUMIFS('Match Records'!E:E, 'Match Records'!B:B, 'Match Records Overview'!A5, 'Match Records'!D:D, 'Match Records Overview'!D5)</f>
         <v>0</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <f>SUMIFS('Match Records'!F:F, 'Match Records'!B:B, 'Match Records Overview'!A5, 'Match Records'!D:D, 'Match Records Overview'!D5)</f>
         <v>0</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <f>SUMIFS('Match Records'!G:G, 'Match Records'!B:B, 'Match Records Overview'!A5, 'Match Records'!D:D, 'Match Records Overview'!D5)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M5" s="16" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
-        <f>INDEX(Formats!A:A, MATCH(B6, Formats!B:B, 0), 0)</f>
-        <v>40269</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
-      <c r="D6" t="s">
-        <v>27</v>
+        <v>38565</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="12">
+        <v>2</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="E6" t="s">
         <v>36</v>
@@ -1578,32 +1959,42 @@
         <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A6, 'Match Records'!D:D, 'Match Records Overview'!D6, 'Match Records'!H:H, "Draw")</f>
         <v>0</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="14" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J6">
         <f>SUMIFS('Match Records'!E:E, 'Match Records'!B:B, 'Match Records Overview'!A6, 'Match Records'!D:D, 'Match Records Overview'!D6)</f>
         <v>0</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <f>SUMIFS('Match Records'!F:F, 'Match Records'!B:B, 'Match Records Overview'!A6, 'Match Records'!D:D, 'Match Records Overview'!D6)</f>
         <v>0</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <f>SUMIFS('Match Records'!G:G, 'Match Records'!B:B, 'Match Records Overview'!A6, 'Match Records'!D:D, 'Match Records Overview'!D6)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M6" s="16" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
-        <f>INDEX(Formats!A:A, MATCH(B7, Formats!B:B, 0), 0)</f>
-        <v>41821</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" t="s">
-        <v>37</v>
+        <v>38565</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="12">
+        <v>2</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>62</v>
       </c>
       <c r="E7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F7">
         <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A7, 'Match Records'!D:D, 'Match Records Overview'!D7, 'Match Records'!H:H, "Win")</f>
@@ -1617,32 +2008,39 @@
         <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A7, 'Match Records'!D:D, 'Match Records Overview'!D7, 'Match Records'!H:H, "Draw")</f>
         <v>0</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="14" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J7">
         <f>SUMIFS('Match Records'!E:E, 'Match Records'!B:B, 'Match Records Overview'!A7, 'Match Records'!D:D, 'Match Records Overview'!D7)</f>
         <v>0</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <f>SUMIFS('Match Records'!F:F, 'Match Records'!B:B, 'Match Records Overview'!A7, 'Match Records'!D:D, 'Match Records Overview'!D7)</f>
         <v>0</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <f>SUMIFS('Match Records'!G:G, 'Match Records'!B:B, 'Match Records Overview'!A7, 'Match Records'!D:D, 'Match Records Overview'!D7)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M7" s="16" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
-        <f>INDEX(Formats!A:A, MATCH(B8, Formats!B:B, 0), 0)</f>
-        <v>41821</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>5</v>
+        <v>38565</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="12">
+        <v>2</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>67</v>
       </c>
       <c r="E8" t="s">
         <v>36</v>
@@ -1659,32 +2057,39 @@
         <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A8, 'Match Records'!D:D, 'Match Records Overview'!D8, 'Match Records'!H:H, "Draw")</f>
         <v>0</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="14" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J8">
         <f>SUMIFS('Match Records'!E:E, 'Match Records'!B:B, 'Match Records Overview'!A8, 'Match Records'!D:D, 'Match Records Overview'!D8)</f>
         <v>0</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <f>SUMIFS('Match Records'!F:F, 'Match Records'!B:B, 'Match Records Overview'!A8, 'Match Records'!D:D, 'Match Records Overview'!D8)</f>
         <v>0</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <f>SUMIFS('Match Records'!G:G, 'Match Records'!B:B, 'Match Records Overview'!A8, 'Match Records'!D:D, 'Match Records Overview'!D8)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M8" s="16" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
-        <f>INDEX(Formats!A:A, MATCH(B9, Formats!B:B, 0), 0)</f>
-        <v>41821</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>4</v>
+        <v>38565</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="12">
+        <v>2</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>63</v>
       </c>
       <c r="E9" t="s">
         <v>36</v>
@@ -1701,32 +2106,39 @@
         <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A9, 'Match Records'!D:D, 'Match Records Overview'!D9, 'Match Records'!H:H, "Draw")</f>
         <v>0</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="14" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J9">
         <f>SUMIFS('Match Records'!E:E, 'Match Records'!B:B, 'Match Records Overview'!A9, 'Match Records'!D:D, 'Match Records Overview'!D9)</f>
         <v>0</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <f>SUMIFS('Match Records'!F:F, 'Match Records'!B:B, 'Match Records Overview'!A9, 'Match Records'!D:D, 'Match Records Overview'!D9)</f>
         <v>0</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <f>SUMIFS('Match Records'!G:G, 'Match Records'!B:B, 'Match Records Overview'!A9, 'Match Records'!D:D, 'Match Records Overview'!D9)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M9" s="16" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
-        <f>INDEX(Formats!A:A, MATCH(B10, Formats!B:B, 0), 0)</f>
-        <v>41821</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>2</v>
+        <v>38565</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="12">
+        <v>2</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>64</v>
       </c>
       <c r="E10" t="s">
         <v>36</v>
@@ -1743,32 +2155,39 @@
         <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A10, 'Match Records'!D:D, 'Match Records Overview'!D10, 'Match Records'!H:H, "Draw")</f>
         <v>0</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="14" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J10">
         <f>SUMIFS('Match Records'!E:E, 'Match Records'!B:B, 'Match Records Overview'!A10, 'Match Records'!D:D, 'Match Records Overview'!D10)</f>
         <v>0</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <f>SUMIFS('Match Records'!F:F, 'Match Records'!B:B, 'Match Records Overview'!A10, 'Match Records'!D:D, 'Match Records Overview'!D10)</f>
         <v>0</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <f>SUMIFS('Match Records'!G:G, 'Match Records'!B:B, 'Match Records Overview'!A10, 'Match Records'!D:D, 'Match Records Overview'!D10)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M10" s="16" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
-        <f>INDEX(Formats!A:A, MATCH(B11, Formats!B:B, 0), 0)</f>
-        <v>41821</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>6</v>
+        <v>38565</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="12">
+        <v>2</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>68</v>
       </c>
       <c r="E11" t="s">
         <v>36</v>
@@ -1785,32 +2204,39 @@
         <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A11, 'Match Records'!D:D, 'Match Records Overview'!D11, 'Match Records'!H:H, "Draw")</f>
         <v>0</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="14" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J11">
         <f>SUMIFS('Match Records'!E:E, 'Match Records'!B:B, 'Match Records Overview'!A11, 'Match Records'!D:D, 'Match Records Overview'!D11)</f>
         <v>0</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <f>SUMIFS('Match Records'!F:F, 'Match Records'!B:B, 'Match Records Overview'!A11, 'Match Records'!D:D, 'Match Records Overview'!D11)</f>
         <v>0</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <f>SUMIFS('Match Records'!G:G, 'Match Records'!B:B, 'Match Records Overview'!A11, 'Match Records'!D:D, 'Match Records Overview'!D11)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M11" s="16" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
-        <f>INDEX(Formats!A:A, MATCH(B12, Formats!B:B, 0), 0)</f>
-        <v>41821</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12" t="s">
-        <v>7</v>
+        <v>38565</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="12">
+        <v>2</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="E12" t="s">
         <v>36</v>
@@ -1827,32 +2253,40 @@
         <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A12, 'Match Records'!D:D, 'Match Records Overview'!D12, 'Match Records'!H:H, "Draw")</f>
         <v>0</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="14" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J12">
         <f>SUMIFS('Match Records'!E:E, 'Match Records'!B:B, 'Match Records Overview'!A12, 'Match Records'!D:D, 'Match Records Overview'!D12)</f>
         <v>0</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <f>SUMIFS('Match Records'!F:F, 'Match Records'!B:B, 'Match Records Overview'!A12, 'Match Records'!D:D, 'Match Records Overview'!D12)</f>
         <v>0</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <f>SUMIFS('Match Records'!G:G, 'Match Records'!B:B, 'Match Records Overview'!A12, 'Match Records'!D:D, 'Match Records Overview'!D12)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M12" s="16" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <f>INDEX(Formats!A:A, MATCH(B13, Formats!B:B, 0), 0)</f>
-        <v>41821</v>
+        <v>40269</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="C13">
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="E13" t="s">
         <v>36</v>
@@ -1869,32 +2303,40 @@
         <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A13, 'Match Records'!D:D, 'Match Records Overview'!D13, 'Match Records'!H:H, "Draw")</f>
         <v>0</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="14" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J13">
         <f>SUMIFS('Match Records'!E:E, 'Match Records'!B:B, 'Match Records Overview'!A13, 'Match Records'!D:D, 'Match Records Overview'!D13)</f>
         <v>0</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <f>SUMIFS('Match Records'!F:F, 'Match Records'!B:B, 'Match Records Overview'!A13, 'Match Records'!D:D, 'Match Records Overview'!D13)</f>
         <v>0</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <f>SUMIFS('Match Records'!G:G, 'Match Records'!B:B, 'Match Records Overview'!A13, 'Match Records'!D:D, 'Match Records Overview'!D13)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M13" s="16" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <f>INDEX(Formats!A:A, MATCH(B14, Formats!B:B, 0), 0)</f>
-        <v>41821</v>
+        <v>40269</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="C14">
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="E14" t="s">
         <v>36</v>
@@ -1911,32 +2353,40 @@
         <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A14, 'Match Records'!D:D, 'Match Records Overview'!D14, 'Match Records'!H:H, "Draw")</f>
         <v>0</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="14" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J14">
         <f>SUMIFS('Match Records'!E:E, 'Match Records'!B:B, 'Match Records Overview'!A14, 'Match Records'!D:D, 'Match Records Overview'!D14)</f>
         <v>0</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <f>SUMIFS('Match Records'!F:F, 'Match Records'!B:B, 'Match Records Overview'!A14, 'Match Records'!D:D, 'Match Records Overview'!D14)</f>
         <v>0</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <f>SUMIFS('Match Records'!G:G, 'Match Records'!B:B, 'Match Records Overview'!A14, 'Match Records'!D:D, 'Match Records Overview'!D14)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M14" s="16" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <f>INDEX(Formats!A:A, MATCH(B15, Formats!B:B, 0), 0)</f>
-        <v>41821</v>
+        <v>40269</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="C15">
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="E15" t="s">
         <v>36</v>
@@ -1953,32 +2403,40 @@
         <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A15, 'Match Records'!D:D, 'Match Records Overview'!D15, 'Match Records'!H:H, "Draw")</f>
         <v>0</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="14" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J15">
         <f>SUMIFS('Match Records'!E:E, 'Match Records'!B:B, 'Match Records Overview'!A15, 'Match Records'!D:D, 'Match Records Overview'!D15)</f>
         <v>0</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <f>SUMIFS('Match Records'!F:F, 'Match Records'!B:B, 'Match Records Overview'!A15, 'Match Records'!D:D, 'Match Records Overview'!D15)</f>
         <v>0</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <f>SUMIFS('Match Records'!G:G, 'Match Records'!B:B, 'Match Records Overview'!A15, 'Match Records'!D:D, 'Match Records Overview'!D15)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M15" s="16" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <f>INDEX(Formats!A:A, MATCH(B16, Formats!B:B, 0), 0)</f>
-        <v>41821</v>
+        <v>40269</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="C16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D16" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="E16" t="s">
         <v>36</v>
@@ -1995,32 +2453,40 @@
         <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A16, 'Match Records'!D:D, 'Match Records Overview'!D16, 'Match Records'!H:H, "Draw")</f>
         <v>0</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="14" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J16">
         <f>SUMIFS('Match Records'!E:E, 'Match Records'!B:B, 'Match Records Overview'!A16, 'Match Records'!D:D, 'Match Records Overview'!D16)</f>
         <v>0</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <f>SUMIFS('Match Records'!F:F, 'Match Records'!B:B, 'Match Records Overview'!A16, 'Match Records'!D:D, 'Match Records Overview'!D16)</f>
         <v>0</v>
       </c>
-      <c r="K16">
+      <c r="L16">
         <f>SUMIFS('Match Records'!G:G, 'Match Records'!B:B, 'Match Records Overview'!A16, 'Match Records'!D:D, 'Match Records Overview'!D16)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M16" s="16" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <f>INDEX(Formats!A:A, MATCH(B17, Formats!B:B, 0), 0)</f>
-        <v>41821</v>
+        <v>40269</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="C17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D17" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="E17" t="s">
         <v>36</v>
@@ -2037,20 +2503,28 @@
         <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A17, 'Match Records'!D:D, 'Match Records Overview'!D17, 'Match Records'!H:H, "Draw")</f>
         <v>0</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="14" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J17">
         <f>SUMIFS('Match Records'!E:E, 'Match Records'!B:B, 'Match Records Overview'!A17, 'Match Records'!D:D, 'Match Records Overview'!D17)</f>
         <v>0</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <f>SUMIFS('Match Records'!F:F, 'Match Records'!B:B, 'Match Records Overview'!A17, 'Match Records'!D:D, 'Match Records Overview'!D17)</f>
         <v>0</v>
       </c>
-      <c r="K17">
+      <c r="L17">
         <f>SUMIFS('Match Records'!G:G, 'Match Records'!B:B, 'Match Records Overview'!A17, 'Match Records'!D:D, 'Match Records Overview'!D17)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M17" s="16" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <f>INDEX(Formats!A:A, MATCH(B18, Formats!B:B, 0), 0)</f>
         <v>41821</v>
@@ -2058,14 +2532,11 @@
       <c r="B18" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C18">
-        <v>2</v>
-      </c>
       <c r="D18" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="E18" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F18">
         <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A18, 'Match Records'!D:D, 'Match Records Overview'!D18, 'Match Records'!H:H, "Win")</f>
@@ -2079,20 +2550,28 @@
         <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A18, 'Match Records'!D:D, 'Match Records Overview'!D18, 'Match Records'!H:H, "Draw")</f>
         <v>0</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="14" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J18">
         <f>SUMIFS('Match Records'!E:E, 'Match Records'!B:B, 'Match Records Overview'!A18, 'Match Records'!D:D, 'Match Records Overview'!D18)</f>
         <v>0</v>
       </c>
-      <c r="J18">
+      <c r="K18">
         <f>SUMIFS('Match Records'!F:F, 'Match Records'!B:B, 'Match Records Overview'!A18, 'Match Records'!D:D, 'Match Records Overview'!D18)</f>
         <v>0</v>
       </c>
-      <c r="K18">
+      <c r="L18">
         <f>SUMIFS('Match Records'!G:G, 'Match Records'!B:B, 'Match Records Overview'!A18, 'Match Records'!D:D, 'Match Records Overview'!D18)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M18" s="16" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <f>INDEX(Formats!A:A, MATCH(B19, Formats!B:B, 0), 0)</f>
         <v>41821</v>
@@ -2101,10 +2580,10 @@
         <v>2</v>
       </c>
       <c r="C19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="E19" t="s">
         <v>36</v>
@@ -2121,20 +2600,28 @@
         <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A19, 'Match Records'!D:D, 'Match Records Overview'!D19, 'Match Records'!H:H, "Draw")</f>
         <v>0</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="14" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J19">
         <f>SUMIFS('Match Records'!E:E, 'Match Records'!B:B, 'Match Records Overview'!A19, 'Match Records'!D:D, 'Match Records Overview'!D19)</f>
         <v>0</v>
       </c>
-      <c r="J19">
+      <c r="K19">
         <f>SUMIFS('Match Records'!F:F, 'Match Records'!B:B, 'Match Records Overview'!A19, 'Match Records'!D:D, 'Match Records Overview'!D19)</f>
         <v>0</v>
       </c>
-      <c r="K19">
+      <c r="L19">
         <f>SUMIFS('Match Records'!G:G, 'Match Records'!B:B, 'Match Records Overview'!A19, 'Match Records'!D:D, 'Match Records Overview'!D19)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M19" s="16" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <f>INDEX(Formats!A:A, MATCH(B20, Formats!B:B, 0), 0)</f>
         <v>41821</v>
@@ -2143,10 +2630,10 @@
         <v>2</v>
       </c>
       <c r="C20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="E20" t="s">
         <v>36</v>
@@ -2163,20 +2650,28 @@
         <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A20, 'Match Records'!D:D, 'Match Records Overview'!D20, 'Match Records'!H:H, "Draw")</f>
         <v>0</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="14" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J20">
         <f>SUMIFS('Match Records'!E:E, 'Match Records'!B:B, 'Match Records Overview'!A20, 'Match Records'!D:D, 'Match Records Overview'!D20)</f>
         <v>0</v>
       </c>
-      <c r="J20">
+      <c r="K20">
         <f>SUMIFS('Match Records'!F:F, 'Match Records'!B:B, 'Match Records Overview'!A20, 'Match Records'!D:D, 'Match Records Overview'!D20)</f>
         <v>0</v>
       </c>
-      <c r="K20">
+      <c r="L20">
         <f>SUMIFS('Match Records'!G:G, 'Match Records'!B:B, 'Match Records Overview'!A20, 'Match Records'!D:D, 'Match Records Overview'!D20)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M20" s="16" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <f>INDEX(Formats!A:A, MATCH(B21, Formats!B:B, 0), 0)</f>
         <v>41821</v>
@@ -2185,10 +2680,10 @@
         <v>2</v>
       </c>
       <c r="C21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E21" t="s">
         <v>36</v>
@@ -2205,20 +2700,28 @@
         <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A21, 'Match Records'!D:D, 'Match Records Overview'!D21, 'Match Records'!H:H, "Draw")</f>
         <v>0</v>
       </c>
-      <c r="I21">
+      <c r="I21" s="14" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J21">
         <f>SUMIFS('Match Records'!E:E, 'Match Records'!B:B, 'Match Records Overview'!A21, 'Match Records'!D:D, 'Match Records Overview'!D21)</f>
         <v>0</v>
       </c>
-      <c r="J21">
+      <c r="K21">
         <f>SUMIFS('Match Records'!F:F, 'Match Records'!B:B, 'Match Records Overview'!A21, 'Match Records'!D:D, 'Match Records Overview'!D21)</f>
         <v>0</v>
       </c>
-      <c r="K21">
+      <c r="L21">
         <f>SUMIFS('Match Records'!G:G, 'Match Records'!B:B, 'Match Records Overview'!A21, 'Match Records'!D:D, 'Match Records Overview'!D21)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M21" s="16" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <f>INDEX(Formats!A:A, MATCH(B22, Formats!B:B, 0), 0)</f>
         <v>41821</v>
@@ -2227,10 +2730,10 @@
         <v>2</v>
       </c>
       <c r="C22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="E22" t="s">
         <v>36</v>
@@ -2247,20 +2750,28 @@
         <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A22, 'Match Records'!D:D, 'Match Records Overview'!D22, 'Match Records'!H:H, "Draw")</f>
         <v>0</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="14" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J22">
         <f>SUMIFS('Match Records'!E:E, 'Match Records'!B:B, 'Match Records Overview'!A22, 'Match Records'!D:D, 'Match Records Overview'!D22)</f>
         <v>0</v>
       </c>
-      <c r="J22">
+      <c r="K22">
         <f>SUMIFS('Match Records'!F:F, 'Match Records'!B:B, 'Match Records Overview'!A22, 'Match Records'!D:D, 'Match Records Overview'!D22)</f>
         <v>0</v>
       </c>
-      <c r="K22">
+      <c r="L22">
         <f>SUMIFS('Match Records'!G:G, 'Match Records'!B:B, 'Match Records Overview'!A22, 'Match Records'!D:D, 'Match Records Overview'!D22)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M22" s="16" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <f>INDEX(Formats!A:A, MATCH(B23, Formats!B:B, 0), 0)</f>
         <v>41821</v>
@@ -2269,10 +2780,10 @@
         <v>2</v>
       </c>
       <c r="C23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="E23" t="s">
         <v>36</v>
@@ -2289,20 +2800,28 @@
         <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A23, 'Match Records'!D:D, 'Match Records Overview'!D23, 'Match Records'!H:H, "Draw")</f>
         <v>0</v>
       </c>
-      <c r="I23">
+      <c r="I23" s="14" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J23">
         <f>SUMIFS('Match Records'!E:E, 'Match Records'!B:B, 'Match Records Overview'!A23, 'Match Records'!D:D, 'Match Records Overview'!D23)</f>
         <v>0</v>
       </c>
-      <c r="J23">
+      <c r="K23">
         <f>SUMIFS('Match Records'!F:F, 'Match Records'!B:B, 'Match Records Overview'!A23, 'Match Records'!D:D, 'Match Records Overview'!D23)</f>
         <v>0</v>
       </c>
-      <c r="K23">
+      <c r="L23">
         <f>SUMIFS('Match Records'!G:G, 'Match Records'!B:B, 'Match Records Overview'!A23, 'Match Records'!D:D, 'Match Records Overview'!D23)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M23" s="16" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <f>INDEX(Formats!A:A, MATCH(B24, Formats!B:B, 0), 0)</f>
         <v>41821</v>
@@ -2314,7 +2833,7 @@
         <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="E24" t="s">
         <v>36</v>
@@ -2331,20 +2850,28 @@
         <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A24, 'Match Records'!D:D, 'Match Records Overview'!D24, 'Match Records'!H:H, "Draw")</f>
         <v>0</v>
       </c>
-      <c r="I24">
+      <c r="I24" s="14" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J24">
         <f>SUMIFS('Match Records'!E:E, 'Match Records'!B:B, 'Match Records Overview'!A24, 'Match Records'!D:D, 'Match Records Overview'!D24)</f>
         <v>0</v>
       </c>
-      <c r="J24">
+      <c r="K24">
         <f>SUMIFS('Match Records'!F:F, 'Match Records'!B:B, 'Match Records Overview'!A24, 'Match Records'!D:D, 'Match Records Overview'!D24)</f>
         <v>0</v>
       </c>
-      <c r="K24">
+      <c r="L24">
         <f>SUMIFS('Match Records'!G:G, 'Match Records'!B:B, 'Match Records Overview'!A24, 'Match Records'!D:D, 'Match Records Overview'!D24)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M24" s="16" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <f>INDEX(Formats!A:A, MATCH(B25, Formats!B:B, 0), 0)</f>
         <v>41821</v>
@@ -2356,7 +2883,7 @@
         <v>2</v>
       </c>
       <c r="D25" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E25" t="s">
         <v>36</v>
@@ -2373,25 +2900,583 @@
         <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A25, 'Match Records'!D:D, 'Match Records Overview'!D25, 'Match Records'!H:H, "Draw")</f>
         <v>0</v>
       </c>
-      <c r="I25">
+      <c r="I25" s="14" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J25">
         <f>SUMIFS('Match Records'!E:E, 'Match Records'!B:B, 'Match Records Overview'!A25, 'Match Records'!D:D, 'Match Records Overview'!D25)</f>
         <v>0</v>
       </c>
-      <c r="J25">
+      <c r="K25">
         <f>SUMIFS('Match Records'!F:F, 'Match Records'!B:B, 'Match Records Overview'!A25, 'Match Records'!D:D, 'Match Records Overview'!D25)</f>
         <v>0</v>
       </c>
-      <c r="K25">
+      <c r="L25">
         <f>SUMIFS('Match Records'!G:G, 'Match Records'!B:B, 'Match Records Overview'!A25, 'Match Records'!D:D, 'Match Records Overview'!D25)</f>
         <v>0</v>
       </c>
+      <c r="M25" s="16" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <f>INDEX(Formats!A:A, MATCH(B26, Formats!B:B, 0), 0)</f>
+        <v>41821</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" t="s">
+        <v>36</v>
+      </c>
+      <c r="F26">
+        <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A26, 'Match Records'!D:D, 'Match Records Overview'!D26, 'Match Records'!H:H, "Win")</f>
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A26, 'Match Records'!D:D, 'Match Records Overview'!D26, 'Match Records'!H:H, "Lose")</f>
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A26, 'Match Records'!D:D, 'Match Records Overview'!D26, 'Match Records'!H:H, "Draw")</f>
+        <v>0</v>
+      </c>
+      <c r="I26" s="14" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J26">
+        <f>SUMIFS('Match Records'!E:E, 'Match Records'!B:B, 'Match Records Overview'!A26, 'Match Records'!D:D, 'Match Records Overview'!D26)</f>
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <f>SUMIFS('Match Records'!F:F, 'Match Records'!B:B, 'Match Records Overview'!A26, 'Match Records'!D:D, 'Match Records Overview'!D26)</f>
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <f>SUMIFS('Match Records'!G:G, 'Match Records'!B:B, 'Match Records Overview'!A26, 'Match Records'!D:D, 'Match Records Overview'!D26)</f>
+        <v>0</v>
+      </c>
+      <c r="M26" s="16" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <f>INDEX(Formats!A:A, MATCH(B27, Formats!B:B, 0), 0)</f>
+        <v>41821</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" t="s">
+        <v>36</v>
+      </c>
+      <c r="F27">
+        <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A27, 'Match Records'!D:D, 'Match Records Overview'!D27, 'Match Records'!H:H, "Win")</f>
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A27, 'Match Records'!D:D, 'Match Records Overview'!D27, 'Match Records'!H:H, "Lose")</f>
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A27, 'Match Records'!D:D, 'Match Records Overview'!D27, 'Match Records'!H:H, "Draw")</f>
+        <v>0</v>
+      </c>
+      <c r="I27" s="14" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J27">
+        <f>SUMIFS('Match Records'!E:E, 'Match Records'!B:B, 'Match Records Overview'!A27, 'Match Records'!D:D, 'Match Records Overview'!D27)</f>
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <f>SUMIFS('Match Records'!F:F, 'Match Records'!B:B, 'Match Records Overview'!A27, 'Match Records'!D:D, 'Match Records Overview'!D27)</f>
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <f>SUMIFS('Match Records'!G:G, 'Match Records'!B:B, 'Match Records Overview'!A27, 'Match Records'!D:D, 'Match Records Overview'!D27)</f>
+        <v>0</v>
+      </c>
+      <c r="M27" s="16" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <f>INDEX(Formats!A:A, MATCH(B28, Formats!B:B, 0), 0)</f>
+        <v>41821</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" t="s">
+        <v>36</v>
+      </c>
+      <c r="F28">
+        <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A28, 'Match Records'!D:D, 'Match Records Overview'!D28, 'Match Records'!H:H, "Win")</f>
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A28, 'Match Records'!D:D, 'Match Records Overview'!D28, 'Match Records'!H:H, "Lose")</f>
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A28, 'Match Records'!D:D, 'Match Records Overview'!D28, 'Match Records'!H:H, "Draw")</f>
+        <v>0</v>
+      </c>
+      <c r="I28" s="14" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J28">
+        <f>SUMIFS('Match Records'!E:E, 'Match Records'!B:B, 'Match Records Overview'!A28, 'Match Records'!D:D, 'Match Records Overview'!D28)</f>
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <f>SUMIFS('Match Records'!F:F, 'Match Records'!B:B, 'Match Records Overview'!A28, 'Match Records'!D:D, 'Match Records Overview'!D28)</f>
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <f>SUMIFS('Match Records'!G:G, 'Match Records'!B:B, 'Match Records Overview'!A28, 'Match Records'!D:D, 'Match Records Overview'!D28)</f>
+        <v>0</v>
+      </c>
+      <c r="M28" s="16" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <f>INDEX(Formats!A:A, MATCH(B29, Formats!B:B, 0), 0)</f>
+        <v>41821</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" t="s">
+        <v>36</v>
+      </c>
+      <c r="F29">
+        <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A29, 'Match Records'!D:D, 'Match Records Overview'!D29, 'Match Records'!H:H, "Win")</f>
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A29, 'Match Records'!D:D, 'Match Records Overview'!D29, 'Match Records'!H:H, "Lose")</f>
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A29, 'Match Records'!D:D, 'Match Records Overview'!D29, 'Match Records'!H:H, "Draw")</f>
+        <v>0</v>
+      </c>
+      <c r="I29" s="14" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J29">
+        <f>SUMIFS('Match Records'!E:E, 'Match Records'!B:B, 'Match Records Overview'!A29, 'Match Records'!D:D, 'Match Records Overview'!D29)</f>
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <f>SUMIFS('Match Records'!F:F, 'Match Records'!B:B, 'Match Records Overview'!A29, 'Match Records'!D:D, 'Match Records Overview'!D29)</f>
+        <v>0</v>
+      </c>
+      <c r="L29">
+        <f>SUMIFS('Match Records'!G:G, 'Match Records'!B:B, 'Match Records Overview'!A29, 'Match Records'!D:D, 'Match Records Overview'!D29)</f>
+        <v>0</v>
+      </c>
+      <c r="M29" s="16" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <f>INDEX(Formats!A:A, MATCH(B30, Formats!B:B, 0), 0)</f>
+        <v>41821</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="D30" t="s">
+        <v>14</v>
+      </c>
+      <c r="E30" t="s">
+        <v>36</v>
+      </c>
+      <c r="F30">
+        <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A30, 'Match Records'!D:D, 'Match Records Overview'!D30, 'Match Records'!H:H, "Win")</f>
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A30, 'Match Records'!D:D, 'Match Records Overview'!D30, 'Match Records'!H:H, "Lose")</f>
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A30, 'Match Records'!D:D, 'Match Records Overview'!D30, 'Match Records'!H:H, "Draw")</f>
+        <v>0</v>
+      </c>
+      <c r="I30" s="14" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J30">
+        <f>SUMIFS('Match Records'!E:E, 'Match Records'!B:B, 'Match Records Overview'!A30, 'Match Records'!D:D, 'Match Records Overview'!D30)</f>
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <f>SUMIFS('Match Records'!F:F, 'Match Records'!B:B, 'Match Records Overview'!A30, 'Match Records'!D:D, 'Match Records Overview'!D30)</f>
+        <v>0</v>
+      </c>
+      <c r="L30">
+        <f>SUMIFS('Match Records'!G:G, 'Match Records'!B:B, 'Match Records Overview'!A30, 'Match Records'!D:D, 'Match Records Overview'!D30)</f>
+        <v>0</v>
+      </c>
+      <c r="M30" s="16" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <f>INDEX(Formats!A:A, MATCH(B31, Formats!B:B, 0), 0)</f>
+        <v>41821</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" t="s">
+        <v>36</v>
+      </c>
+      <c r="F31">
+        <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A31, 'Match Records'!D:D, 'Match Records Overview'!D31, 'Match Records'!H:H, "Win")</f>
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A31, 'Match Records'!D:D, 'Match Records Overview'!D31, 'Match Records'!H:H, "Lose")</f>
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A31, 'Match Records'!D:D, 'Match Records Overview'!D31, 'Match Records'!H:H, "Draw")</f>
+        <v>0</v>
+      </c>
+      <c r="I31" s="14" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J31">
+        <f>SUMIFS('Match Records'!E:E, 'Match Records'!B:B, 'Match Records Overview'!A31, 'Match Records'!D:D, 'Match Records Overview'!D31)</f>
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <f>SUMIFS('Match Records'!F:F, 'Match Records'!B:B, 'Match Records Overview'!A31, 'Match Records'!D:D, 'Match Records Overview'!D31)</f>
+        <v>0</v>
+      </c>
+      <c r="L31">
+        <f>SUMIFS('Match Records'!G:G, 'Match Records'!B:B, 'Match Records Overview'!A31, 'Match Records'!D:D, 'Match Records Overview'!D31)</f>
+        <v>0</v>
+      </c>
+      <c r="M31" s="16" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
+        <f>INDEX(Formats!A:A, MATCH(B32, Formats!B:B, 0), 0)</f>
+        <v>41821</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="D32" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" t="s">
+        <v>36</v>
+      </c>
+      <c r="F32">
+        <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A32, 'Match Records'!D:D, 'Match Records Overview'!D32, 'Match Records'!H:H, "Win")</f>
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A32, 'Match Records'!D:D, 'Match Records Overview'!D32, 'Match Records'!H:H, "Lose")</f>
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A32, 'Match Records'!D:D, 'Match Records Overview'!D32, 'Match Records'!H:H, "Draw")</f>
+        <v>0</v>
+      </c>
+      <c r="I32" s="14" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J32">
+        <f>SUMIFS('Match Records'!E:E, 'Match Records'!B:B, 'Match Records Overview'!A32, 'Match Records'!D:D, 'Match Records Overview'!D32)</f>
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <f>SUMIFS('Match Records'!F:F, 'Match Records'!B:B, 'Match Records Overview'!A32, 'Match Records'!D:D, 'Match Records Overview'!D32)</f>
+        <v>0</v>
+      </c>
+      <c r="L32">
+        <f>SUMIFS('Match Records'!G:G, 'Match Records'!B:B, 'Match Records Overview'!A32, 'Match Records'!D:D, 'Match Records Overview'!D32)</f>
+        <v>0</v>
+      </c>
+      <c r="M32" s="16" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
+        <f>INDEX(Formats!A:A, MATCH(B33, Formats!B:B, 0), 0)</f>
+        <v>41821</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="D33" t="s">
+        <v>16</v>
+      </c>
+      <c r="E33" t="s">
+        <v>36</v>
+      </c>
+      <c r="F33">
+        <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A33, 'Match Records'!D:D, 'Match Records Overview'!D33, 'Match Records'!H:H, "Win")</f>
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A33, 'Match Records'!D:D, 'Match Records Overview'!D33, 'Match Records'!H:H, "Lose")</f>
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A33, 'Match Records'!D:D, 'Match Records Overview'!D33, 'Match Records'!H:H, "Draw")</f>
+        <v>0</v>
+      </c>
+      <c r="I33" s="14" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J33">
+        <f>SUMIFS('Match Records'!E:E, 'Match Records'!B:B, 'Match Records Overview'!A33, 'Match Records'!D:D, 'Match Records Overview'!D33)</f>
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <f>SUMIFS('Match Records'!F:F, 'Match Records'!B:B, 'Match Records Overview'!A33, 'Match Records'!D:D, 'Match Records Overview'!D33)</f>
+        <v>0</v>
+      </c>
+      <c r="L33">
+        <f>SUMIFS('Match Records'!G:G, 'Match Records'!B:B, 'Match Records Overview'!A33, 'Match Records'!D:D, 'Match Records Overview'!D33)</f>
+        <v>0</v>
+      </c>
+      <c r="M33" s="16" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
+        <f>INDEX(Formats!A:A, MATCH(B34, Formats!B:B, 0), 0)</f>
+        <v>41821</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="D34" t="s">
+        <v>18</v>
+      </c>
+      <c r="E34" t="s">
+        <v>36</v>
+      </c>
+      <c r="F34">
+        <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A34, 'Match Records'!D:D, 'Match Records Overview'!D34, 'Match Records'!H:H, "Win")</f>
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A34, 'Match Records'!D:D, 'Match Records Overview'!D34, 'Match Records'!H:H, "Lose")</f>
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A34, 'Match Records'!D:D, 'Match Records Overview'!D34, 'Match Records'!H:H, "Draw")</f>
+        <v>0</v>
+      </c>
+      <c r="I34" s="14" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J34">
+        <f>SUMIFS('Match Records'!E:E, 'Match Records'!B:B, 'Match Records Overview'!A34, 'Match Records'!D:D, 'Match Records Overview'!D34)</f>
+        <v>0</v>
+      </c>
+      <c r="K34">
+        <f>SUMIFS('Match Records'!F:F, 'Match Records'!B:B, 'Match Records Overview'!A34, 'Match Records'!D:D, 'Match Records Overview'!D34)</f>
+        <v>0</v>
+      </c>
+      <c r="L34">
+        <f>SUMIFS('Match Records'!G:G, 'Match Records'!B:B, 'Match Records Overview'!A34, 'Match Records'!D:D, 'Match Records Overview'!D34)</f>
+        <v>0</v>
+      </c>
+      <c r="M34" s="16" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
+        <f>INDEX(Formats!A:A, MATCH(B35, Formats!B:B, 0), 0)</f>
+        <v>41821</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
+      </c>
+      <c r="D35" t="s">
+        <v>19</v>
+      </c>
+      <c r="E35" t="s">
+        <v>36</v>
+      </c>
+      <c r="F35">
+        <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A35, 'Match Records'!D:D, 'Match Records Overview'!D35, 'Match Records'!H:H, "Win")</f>
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A35, 'Match Records'!D:D, 'Match Records Overview'!D35, 'Match Records'!H:H, "Lose")</f>
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A35, 'Match Records'!D:D, 'Match Records Overview'!D35, 'Match Records'!H:H, "Draw")</f>
+        <v>0</v>
+      </c>
+      <c r="I35" s="14" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J35">
+        <f>SUMIFS('Match Records'!E:E, 'Match Records'!B:B, 'Match Records Overview'!A35, 'Match Records'!D:D, 'Match Records Overview'!D35)</f>
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <f>SUMIFS('Match Records'!F:F, 'Match Records'!B:B, 'Match Records Overview'!A35, 'Match Records'!D:D, 'Match Records Overview'!D35)</f>
+        <v>0</v>
+      </c>
+      <c r="L35">
+        <f>SUMIFS('Match Records'!G:G, 'Match Records'!B:B, 'Match Records Overview'!A35, 'Match Records'!D:D, 'Match Records Overview'!D35)</f>
+        <v>0</v>
+      </c>
+      <c r="M35" s="16" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <f>INDEX(Formats!A:A, MATCH(B36, Formats!B:B, 0), 0)</f>
+        <v>41821</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36">
+        <v>2</v>
+      </c>
+      <c r="D36" t="s">
+        <v>20</v>
+      </c>
+      <c r="E36" t="s">
+        <v>36</v>
+      </c>
+      <c r="F36">
+        <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A36, 'Match Records'!D:D, 'Match Records Overview'!D36, 'Match Records'!H:H, "Win")</f>
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A36, 'Match Records'!D:D, 'Match Records Overview'!D36, 'Match Records'!H:H, "Lose")</f>
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <f>COUNTIFS('Match Records'!B:B, 'Match Records Overview'!A36, 'Match Records'!D:D, 'Match Records Overview'!D36, 'Match Records'!H:H, "Draw")</f>
+        <v>0</v>
+      </c>
+      <c r="I36" s="14" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J36">
+        <f>SUMIFS('Match Records'!E:E, 'Match Records'!B:B, 'Match Records Overview'!A36, 'Match Records'!D:D, 'Match Records Overview'!D36)</f>
+        <v>0</v>
+      </c>
+      <c r="K36">
+        <f>SUMIFS('Match Records'!F:F, 'Match Records'!B:B, 'Match Records Overview'!A36, 'Match Records'!D:D, 'Match Records Overview'!D36)</f>
+        <v>0</v>
+      </c>
+      <c r="L36">
+        <f>SUMIFS('Match Records'!G:G, 'Match Records'!B:B, 'Match Records Overview'!A36, 'Match Records'!D:D, 'Match Records Overview'!D36)</f>
+        <v>0</v>
+      </c>
+      <c r="M36" s="16" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K25">
-    <sortCondition ref="A2:A25"/>
-    <sortCondition ref="E2:E25"/>
-    <sortCondition ref="C2:C25"/>
-    <sortCondition ref="D2:D25"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L36">
+    <sortCondition ref="A13:A36"/>
+    <sortCondition ref="E13:E36"/>
+    <sortCondition ref="C13:C36"/>
+    <sortCondition ref="D13:D36"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2399,10 +3484,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44B7D2B9-9D46-4B9E-9494-05F1699F9F2F}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:I19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2413,12 +3498,14 @@
     <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.42578125" customWidth="1"/>
+    <col min="8" max="8" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="8" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="8" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>34</v>
       </c>
@@ -2438,16 +3525,22 @@
         <v>45</v>
       </c>
       <c r="G1" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="H1" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K1" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <f>INDEX(Formats!A:A, MATCH(B2, Formats!B:B, 0), 0)</f>
         <v>38565</v>
@@ -2460,7 +3553,7 @@
       </c>
       <c r="D2">
         <f>SUMIFS('Match Records Overview'!F:F, 'Match Records Overview'!A:A, 'Format Overview'!A2, 'Match Records Overview'!C:C, 'Format Overview'!C2)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2">
         <f>SUMIFS('Match Records Overview'!G:G, 'Match Records Overview'!A:A, 'Format Overview'!A2, 'Match Records Overview'!C:C, 'Format Overview'!C2)</f>
@@ -2471,19 +3564,27 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <f>SUMIFS('Match Records Overview'!I:I, 'Match Records Overview'!A:A, 'Format Overview'!A2, 'Match Records Overview'!C:C, 'Format Overview'!C2)</f>
-        <v>0</v>
+        <f>D2/SUM(D2+E2)</f>
+        <v>1</v>
       </c>
       <c r="H2">
         <f>SUMIFS('Match Records Overview'!J:J, 'Match Records Overview'!A:A, 'Format Overview'!A2, 'Match Records Overview'!C:C, 'Format Overview'!C2)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I2">
         <f>SUMIFS('Match Records Overview'!K:K, 'Match Records Overview'!A:A, 'Format Overview'!A2, 'Match Records Overview'!C:C, 'Format Overview'!C2)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2">
+        <f>SUMIFS('Match Records Overview'!L:L, 'Match Records Overview'!A:A, 'Format Overview'!A2, 'Match Records Overview'!C:C, 'Format Overview'!C2)</f>
+        <v>0</v>
+      </c>
+      <c r="K2" s="12">
+        <f>H2/SUM(H2+I2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <f>INDEX(Formats!A:A, MATCH(B3, Formats!B:B, 0), 0)</f>
         <v>38565</v>
@@ -2506,9 +3607,9 @@
         <f>SUMIFS('Match Records Overview'!H:H, 'Match Records Overview'!A:A, 'Format Overview'!A3, 'Match Records Overview'!C:C, 'Format Overview'!C3)</f>
         <v>0</v>
       </c>
-      <c r="G3">
-        <f>SUMIFS('Match Records Overview'!I:I, 'Match Records Overview'!A:A, 'Format Overview'!A3, 'Match Records Overview'!C:C, 'Format Overview'!C3)</f>
-        <v>0</v>
+      <c r="G3" t="e">
+        <f t="shared" ref="G3:G19" si="0">D3/SUM(D3+E3)</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="H3">
         <f>SUMIFS('Match Records Overview'!J:J, 'Match Records Overview'!A:A, 'Format Overview'!A3, 'Match Records Overview'!C:C, 'Format Overview'!C3)</f>
@@ -2518,8 +3619,16 @@
         <f>SUMIFS('Match Records Overview'!K:K, 'Match Records Overview'!A:A, 'Format Overview'!A3, 'Match Records Overview'!C:C, 'Format Overview'!C3)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3">
+        <f>SUMIFS('Match Records Overview'!L:L, 'Match Records Overview'!A:A, 'Format Overview'!A3, 'Match Records Overview'!C:C, 'Format Overview'!C3)</f>
+        <v>0</v>
+      </c>
+      <c r="K3" s="12" t="e">
+        <f t="shared" ref="K3:K19" si="1">H3/SUM(H3+I3)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <f>INDEX(Formats!A:A, MATCH(B4, Formats!B:B, 0), 0)</f>
         <v>38565</v>
@@ -2542,9 +3651,9 @@
         <f>SUMIFS('Match Records Overview'!H:H, 'Match Records Overview'!A:A, 'Format Overview'!A4, 'Match Records Overview'!C:C, 'Format Overview'!C4)</f>
         <v>0</v>
       </c>
-      <c r="G4">
-        <f>SUMIFS('Match Records Overview'!I:I, 'Match Records Overview'!A:A, 'Format Overview'!A4, 'Match Records Overview'!C:C, 'Format Overview'!C4)</f>
-        <v>0</v>
+      <c r="G4" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
       </c>
       <c r="H4">
         <f>SUMIFS('Match Records Overview'!J:J, 'Match Records Overview'!A:A, 'Format Overview'!A4, 'Match Records Overview'!C:C, 'Format Overview'!C4)</f>
@@ -2554,8 +3663,16 @@
         <f>SUMIFS('Match Records Overview'!K:K, 'Match Records Overview'!A:A, 'Format Overview'!A4, 'Match Records Overview'!C:C, 'Format Overview'!C4)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4">
+        <f>SUMIFS('Match Records Overview'!L:L, 'Match Records Overview'!A:A, 'Format Overview'!A4, 'Match Records Overview'!C:C, 'Format Overview'!C4)</f>
+        <v>0</v>
+      </c>
+      <c r="K4" s="12" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <f>INDEX(Formats!A:A, MATCH(B5, Formats!B:B, 0), 0)</f>
         <v>39448</v>
@@ -2578,9 +3695,9 @@
         <f>SUMIFS('Match Records Overview'!H:H, 'Match Records Overview'!A:A, 'Format Overview'!A5, 'Match Records Overview'!C:C, 'Format Overview'!C5)</f>
         <v>0</v>
       </c>
-      <c r="G5">
-        <f>SUMIFS('Match Records Overview'!I:I, 'Match Records Overview'!A:A, 'Format Overview'!A5, 'Match Records Overview'!C:C, 'Format Overview'!C5)</f>
-        <v>0</v>
+      <c r="G5" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
       </c>
       <c r="H5">
         <f>SUMIFS('Match Records Overview'!J:J, 'Match Records Overview'!A:A, 'Format Overview'!A5, 'Match Records Overview'!C:C, 'Format Overview'!C5)</f>
@@ -2590,8 +3707,16 @@
         <f>SUMIFS('Match Records Overview'!K:K, 'Match Records Overview'!A:A, 'Format Overview'!A5, 'Match Records Overview'!C:C, 'Format Overview'!C5)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5">
+        <f>SUMIFS('Match Records Overview'!L:L, 'Match Records Overview'!A:A, 'Format Overview'!A5, 'Match Records Overview'!C:C, 'Format Overview'!C5)</f>
+        <v>0</v>
+      </c>
+      <c r="K5" s="12" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <f>INDEX(Formats!A:A, MATCH(B6, Formats!B:B, 0), 0)</f>
         <v>39448</v>
@@ -2614,9 +3739,9 @@
         <f>SUMIFS('Match Records Overview'!H:H, 'Match Records Overview'!A:A, 'Format Overview'!A6, 'Match Records Overview'!C:C, 'Format Overview'!C6)</f>
         <v>0</v>
       </c>
-      <c r="G6">
-        <f>SUMIFS('Match Records Overview'!I:I, 'Match Records Overview'!A:A, 'Format Overview'!A6, 'Match Records Overview'!C:C, 'Format Overview'!C6)</f>
-        <v>0</v>
+      <c r="G6" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
       </c>
       <c r="H6">
         <f>SUMIFS('Match Records Overview'!J:J, 'Match Records Overview'!A:A, 'Format Overview'!A6, 'Match Records Overview'!C:C, 'Format Overview'!C6)</f>
@@ -2626,8 +3751,16 @@
         <f>SUMIFS('Match Records Overview'!K:K, 'Match Records Overview'!A:A, 'Format Overview'!A6, 'Match Records Overview'!C:C, 'Format Overview'!C6)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6">
+        <f>SUMIFS('Match Records Overview'!L:L, 'Match Records Overview'!A:A, 'Format Overview'!A6, 'Match Records Overview'!C:C, 'Format Overview'!C6)</f>
+        <v>0</v>
+      </c>
+      <c r="K6" s="12" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <f>INDEX(Formats!A:A, MATCH(B7, Formats!B:B, 0), 0)</f>
         <v>39448</v>
@@ -2650,9 +3783,9 @@
         <f>SUMIFS('Match Records Overview'!H:H, 'Match Records Overview'!A:A, 'Format Overview'!A7, 'Match Records Overview'!C:C, 'Format Overview'!C7)</f>
         <v>0</v>
       </c>
-      <c r="G7">
-        <f>SUMIFS('Match Records Overview'!I:I, 'Match Records Overview'!A:A, 'Format Overview'!A7, 'Match Records Overview'!C:C, 'Format Overview'!C7)</f>
-        <v>0</v>
+      <c r="G7" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
       </c>
       <c r="H7">
         <f>SUMIFS('Match Records Overview'!J:J, 'Match Records Overview'!A:A, 'Format Overview'!A7, 'Match Records Overview'!C:C, 'Format Overview'!C7)</f>
@@ -2662,8 +3795,16 @@
         <f>SUMIFS('Match Records Overview'!K:K, 'Match Records Overview'!A:A, 'Format Overview'!A7, 'Match Records Overview'!C:C, 'Format Overview'!C7)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7">
+        <f>SUMIFS('Match Records Overview'!L:L, 'Match Records Overview'!A:A, 'Format Overview'!A7, 'Match Records Overview'!C:C, 'Format Overview'!C7)</f>
+        <v>0</v>
+      </c>
+      <c r="K7" s="12" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <f>INDEX(Formats!A:A, MATCH(B8, Formats!B:B, 0), 0)</f>
         <v>39630</v>
@@ -2686,9 +3827,9 @@
         <f>SUMIFS('Match Records Overview'!H:H, 'Match Records Overview'!A:A, 'Format Overview'!A8, 'Match Records Overview'!C:C, 'Format Overview'!C8)</f>
         <v>0</v>
       </c>
-      <c r="G8">
-        <f>SUMIFS('Match Records Overview'!I:I, 'Match Records Overview'!A:A, 'Format Overview'!A8, 'Match Records Overview'!C:C, 'Format Overview'!C8)</f>
-        <v>0</v>
+      <c r="G8" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
       </c>
       <c r="H8">
         <f>SUMIFS('Match Records Overview'!J:J, 'Match Records Overview'!A:A, 'Format Overview'!A8, 'Match Records Overview'!C:C, 'Format Overview'!C8)</f>
@@ -2698,8 +3839,16 @@
         <f>SUMIFS('Match Records Overview'!K:K, 'Match Records Overview'!A:A, 'Format Overview'!A8, 'Match Records Overview'!C:C, 'Format Overview'!C8)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <f>SUMIFS('Match Records Overview'!L:L, 'Match Records Overview'!A:A, 'Format Overview'!A8, 'Match Records Overview'!C:C, 'Format Overview'!C8)</f>
+        <v>0</v>
+      </c>
+      <c r="K8" s="12" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <f>INDEX(Formats!A:A, MATCH(B9, Formats!B:B, 0), 0)</f>
         <v>39630</v>
@@ -2722,9 +3871,9 @@
         <f>SUMIFS('Match Records Overview'!H:H, 'Match Records Overview'!A:A, 'Format Overview'!A9, 'Match Records Overview'!C:C, 'Format Overview'!C9)</f>
         <v>0</v>
       </c>
-      <c r="G9">
-        <f>SUMIFS('Match Records Overview'!I:I, 'Match Records Overview'!A:A, 'Format Overview'!A9, 'Match Records Overview'!C:C, 'Format Overview'!C9)</f>
-        <v>0</v>
+      <c r="G9" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
       </c>
       <c r="H9">
         <f>SUMIFS('Match Records Overview'!J:J, 'Match Records Overview'!A:A, 'Format Overview'!A9, 'Match Records Overview'!C:C, 'Format Overview'!C9)</f>
@@ -2734,8 +3883,16 @@
         <f>SUMIFS('Match Records Overview'!K:K, 'Match Records Overview'!A:A, 'Format Overview'!A9, 'Match Records Overview'!C:C, 'Format Overview'!C9)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9">
+        <f>SUMIFS('Match Records Overview'!L:L, 'Match Records Overview'!A:A, 'Format Overview'!A9, 'Match Records Overview'!C:C, 'Format Overview'!C9)</f>
+        <v>0</v>
+      </c>
+      <c r="K9" s="12" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <f>INDEX(Formats!A:A, MATCH(B10, Formats!B:B, 0), 0)</f>
         <v>39630</v>
@@ -2758,9 +3915,9 @@
         <f>SUMIFS('Match Records Overview'!H:H, 'Match Records Overview'!A:A, 'Format Overview'!A10, 'Match Records Overview'!C:C, 'Format Overview'!C10)</f>
         <v>0</v>
       </c>
-      <c r="G10">
-        <f>SUMIFS('Match Records Overview'!I:I, 'Match Records Overview'!A:A, 'Format Overview'!A10, 'Match Records Overview'!C:C, 'Format Overview'!C10)</f>
-        <v>0</v>
+      <c r="G10" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
       </c>
       <c r="H10">
         <f>SUMIFS('Match Records Overview'!J:J, 'Match Records Overview'!A:A, 'Format Overview'!A10, 'Match Records Overview'!C:C, 'Format Overview'!C10)</f>
@@ -2770,8 +3927,16 @@
         <f>SUMIFS('Match Records Overview'!K:K, 'Match Records Overview'!A:A, 'Format Overview'!A10, 'Match Records Overview'!C:C, 'Format Overview'!C10)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <f>SUMIFS('Match Records Overview'!L:L, 'Match Records Overview'!A:A, 'Format Overview'!A10, 'Match Records Overview'!C:C, 'Format Overview'!C10)</f>
+        <v>0</v>
+      </c>
+      <c r="K10" s="12" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <f>INDEX(Formats!A:A, MATCH(B11, Formats!B:B, 0), 0)</f>
         <v>40269</v>
@@ -2794,9 +3959,9 @@
         <f>SUMIFS('Match Records Overview'!H:H, 'Match Records Overview'!A:A, 'Format Overview'!A11, 'Match Records Overview'!C:C, 'Format Overview'!C11)</f>
         <v>0</v>
       </c>
-      <c r="G11">
-        <f>SUMIFS('Match Records Overview'!I:I, 'Match Records Overview'!A:A, 'Format Overview'!A11, 'Match Records Overview'!C:C, 'Format Overview'!C11)</f>
-        <v>0</v>
+      <c r="G11" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
       </c>
       <c r="H11">
         <f>SUMIFS('Match Records Overview'!J:J, 'Match Records Overview'!A:A, 'Format Overview'!A11, 'Match Records Overview'!C:C, 'Format Overview'!C11)</f>
@@ -2806,8 +3971,16 @@
         <f>SUMIFS('Match Records Overview'!K:K, 'Match Records Overview'!A:A, 'Format Overview'!A11, 'Match Records Overview'!C:C, 'Format Overview'!C11)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11">
+        <f>SUMIFS('Match Records Overview'!L:L, 'Match Records Overview'!A:A, 'Format Overview'!A11, 'Match Records Overview'!C:C, 'Format Overview'!C11)</f>
+        <v>0</v>
+      </c>
+      <c r="K11" s="12" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <f>INDEX(Formats!A:A, MATCH(B12, Formats!B:B, 0), 0)</f>
         <v>40269</v>
@@ -2830,9 +4003,9 @@
         <f>SUMIFS('Match Records Overview'!H:H, 'Match Records Overview'!A:A, 'Format Overview'!A12, 'Match Records Overview'!C:C, 'Format Overview'!C12)</f>
         <v>0</v>
       </c>
-      <c r="G12">
-        <f>SUMIFS('Match Records Overview'!I:I, 'Match Records Overview'!A:A, 'Format Overview'!A12, 'Match Records Overview'!C:C, 'Format Overview'!C12)</f>
-        <v>0</v>
+      <c r="G12" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
       </c>
       <c r="H12">
         <f>SUMIFS('Match Records Overview'!J:J, 'Match Records Overview'!A:A, 'Format Overview'!A12, 'Match Records Overview'!C:C, 'Format Overview'!C12)</f>
@@ -2842,8 +4015,16 @@
         <f>SUMIFS('Match Records Overview'!K:K, 'Match Records Overview'!A:A, 'Format Overview'!A12, 'Match Records Overview'!C:C, 'Format Overview'!C12)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12">
+        <f>SUMIFS('Match Records Overview'!L:L, 'Match Records Overview'!A:A, 'Format Overview'!A12, 'Match Records Overview'!C:C, 'Format Overview'!C12)</f>
+        <v>0</v>
+      </c>
+      <c r="K12" s="12" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <f>INDEX(Formats!A:A, MATCH(B13, Formats!B:B, 0), 0)</f>
         <v>40269</v>
@@ -2866,9 +4047,9 @@
         <f>SUMIFS('Match Records Overview'!H:H, 'Match Records Overview'!A:A, 'Format Overview'!A13, 'Match Records Overview'!C:C, 'Format Overview'!C13)</f>
         <v>0</v>
       </c>
-      <c r="G13">
-        <f>SUMIFS('Match Records Overview'!I:I, 'Match Records Overview'!A:A, 'Format Overview'!A13, 'Match Records Overview'!C:C, 'Format Overview'!C13)</f>
-        <v>0</v>
+      <c r="G13" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
       </c>
       <c r="H13">
         <f>SUMIFS('Match Records Overview'!J:J, 'Match Records Overview'!A:A, 'Format Overview'!A13, 'Match Records Overview'!C:C, 'Format Overview'!C13)</f>
@@ -2878,8 +4059,16 @@
         <f>SUMIFS('Match Records Overview'!K:K, 'Match Records Overview'!A:A, 'Format Overview'!A13, 'Match Records Overview'!C:C, 'Format Overview'!C13)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13">
+        <f>SUMIFS('Match Records Overview'!L:L, 'Match Records Overview'!A:A, 'Format Overview'!A13, 'Match Records Overview'!C:C, 'Format Overview'!C13)</f>
+        <v>0</v>
+      </c>
+      <c r="K13" s="12" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <f>INDEX(Formats!A:A, MATCH(B14, Formats!B:B, 0), 0)</f>
         <v>40817</v>
@@ -2902,9 +4091,9 @@
         <f>SUMIFS('Match Records Overview'!H:H, 'Match Records Overview'!A:A, 'Format Overview'!A14, 'Match Records Overview'!C:C, 'Format Overview'!C14)</f>
         <v>0</v>
       </c>
-      <c r="G14">
-        <f>SUMIFS('Match Records Overview'!I:I, 'Match Records Overview'!A:A, 'Format Overview'!A14, 'Match Records Overview'!C:C, 'Format Overview'!C14)</f>
-        <v>0</v>
+      <c r="G14" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
       </c>
       <c r="H14">
         <f>SUMIFS('Match Records Overview'!J:J, 'Match Records Overview'!A:A, 'Format Overview'!A14, 'Match Records Overview'!C:C, 'Format Overview'!C14)</f>
@@ -2914,8 +4103,16 @@
         <f>SUMIFS('Match Records Overview'!K:K, 'Match Records Overview'!A:A, 'Format Overview'!A14, 'Match Records Overview'!C:C, 'Format Overview'!C14)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14">
+        <f>SUMIFS('Match Records Overview'!L:L, 'Match Records Overview'!A:A, 'Format Overview'!A14, 'Match Records Overview'!C:C, 'Format Overview'!C14)</f>
+        <v>0</v>
+      </c>
+      <c r="K14" s="12" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <f>INDEX(Formats!A:A, MATCH(B15, Formats!B:B, 0), 0)</f>
         <v>40817</v>
@@ -2938,9 +4135,9 @@
         <f>SUMIFS('Match Records Overview'!H:H, 'Match Records Overview'!A:A, 'Format Overview'!A15, 'Match Records Overview'!C:C, 'Format Overview'!C15)</f>
         <v>0</v>
       </c>
-      <c r="G15">
-        <f>SUMIFS('Match Records Overview'!I:I, 'Match Records Overview'!A:A, 'Format Overview'!A15, 'Match Records Overview'!C:C, 'Format Overview'!C15)</f>
-        <v>0</v>
+      <c r="G15" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
       </c>
       <c r="H15">
         <f>SUMIFS('Match Records Overview'!J:J, 'Match Records Overview'!A:A, 'Format Overview'!A15, 'Match Records Overview'!C:C, 'Format Overview'!C15)</f>
@@ -2950,8 +4147,16 @@
         <f>SUMIFS('Match Records Overview'!K:K, 'Match Records Overview'!A:A, 'Format Overview'!A15, 'Match Records Overview'!C:C, 'Format Overview'!C15)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15">
+        <f>SUMIFS('Match Records Overview'!L:L, 'Match Records Overview'!A:A, 'Format Overview'!A15, 'Match Records Overview'!C:C, 'Format Overview'!C15)</f>
+        <v>0</v>
+      </c>
+      <c r="K15" s="12" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <f>INDEX(Formats!A:A, MATCH(B16, Formats!B:B, 0), 0)</f>
         <v>40817</v>
@@ -2974,9 +4179,9 @@
         <f>SUMIFS('Match Records Overview'!H:H, 'Match Records Overview'!A:A, 'Format Overview'!A16, 'Match Records Overview'!C:C, 'Format Overview'!C16)</f>
         <v>0</v>
       </c>
-      <c r="G16">
-        <f>SUMIFS('Match Records Overview'!I:I, 'Match Records Overview'!A:A, 'Format Overview'!A16, 'Match Records Overview'!C:C, 'Format Overview'!C16)</f>
-        <v>0</v>
+      <c r="G16" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
       </c>
       <c r="H16">
         <f>SUMIFS('Match Records Overview'!J:J, 'Match Records Overview'!A:A, 'Format Overview'!A16, 'Match Records Overview'!C:C, 'Format Overview'!C16)</f>
@@ -2986,8 +4191,16 @@
         <f>SUMIFS('Match Records Overview'!K:K, 'Match Records Overview'!A:A, 'Format Overview'!A16, 'Match Records Overview'!C:C, 'Format Overview'!C16)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16">
+        <f>SUMIFS('Match Records Overview'!L:L, 'Match Records Overview'!A:A, 'Format Overview'!A16, 'Match Records Overview'!C:C, 'Format Overview'!C16)</f>
+        <v>0</v>
+      </c>
+      <c r="K16" s="12" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <f>INDEX(Formats!A:A, MATCH(B17, Formats!B:B, 0), 0)</f>
         <v>41821</v>
@@ -3010,9 +4223,9 @@
         <f>SUMIFS('Match Records Overview'!H:H, 'Match Records Overview'!A:A, 'Format Overview'!A17, 'Match Records Overview'!C:C, 'Format Overview'!C17)</f>
         <v>0</v>
       </c>
-      <c r="G17">
-        <f>SUMIFS('Match Records Overview'!I:I, 'Match Records Overview'!A:A, 'Format Overview'!A17, 'Match Records Overview'!C:C, 'Format Overview'!C17)</f>
-        <v>0</v>
+      <c r="G17" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
       </c>
       <c r="H17">
         <f>SUMIFS('Match Records Overview'!J:J, 'Match Records Overview'!A:A, 'Format Overview'!A17, 'Match Records Overview'!C:C, 'Format Overview'!C17)</f>
@@ -3022,8 +4235,16 @@
         <f>SUMIFS('Match Records Overview'!K:K, 'Match Records Overview'!A:A, 'Format Overview'!A17, 'Match Records Overview'!C:C, 'Format Overview'!C17)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17">
+        <f>SUMIFS('Match Records Overview'!L:L, 'Match Records Overview'!A:A, 'Format Overview'!A17, 'Match Records Overview'!C:C, 'Format Overview'!C17)</f>
+        <v>0</v>
+      </c>
+      <c r="K17" s="12" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <f>INDEX(Formats!A:A, MATCH(B18, Formats!B:B, 0), 0)</f>
         <v>41821</v>
@@ -3046,9 +4267,9 @@
         <f>SUMIFS('Match Records Overview'!H:H, 'Match Records Overview'!A:A, 'Format Overview'!A18, 'Match Records Overview'!C:C, 'Format Overview'!C18)</f>
         <v>0</v>
       </c>
-      <c r="G18">
-        <f>SUMIFS('Match Records Overview'!I:I, 'Match Records Overview'!A:A, 'Format Overview'!A18, 'Match Records Overview'!C:C, 'Format Overview'!C18)</f>
-        <v>0</v>
+      <c r="G18" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
       </c>
       <c r="H18">
         <f>SUMIFS('Match Records Overview'!J:J, 'Match Records Overview'!A:A, 'Format Overview'!A18, 'Match Records Overview'!C:C, 'Format Overview'!C18)</f>
@@ -3058,8 +4279,16 @@
         <f>SUMIFS('Match Records Overview'!K:K, 'Match Records Overview'!A:A, 'Format Overview'!A18, 'Match Records Overview'!C:C, 'Format Overview'!C18)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18">
+        <f>SUMIFS('Match Records Overview'!L:L, 'Match Records Overview'!A:A, 'Format Overview'!A18, 'Match Records Overview'!C:C, 'Format Overview'!C18)</f>
+        <v>0</v>
+      </c>
+      <c r="K18" s="12" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <f>INDEX(Formats!A:A, MATCH(B19, Formats!B:B, 0), 0)</f>
         <v>41821</v>
@@ -3082,9 +4311,9 @@
         <f>SUMIFS('Match Records Overview'!H:H, 'Match Records Overview'!A:A, 'Format Overview'!A19, 'Match Records Overview'!C:C, 'Format Overview'!C19)</f>
         <v>0</v>
       </c>
-      <c r="G19">
-        <f>SUMIFS('Match Records Overview'!I:I, 'Match Records Overview'!A:A, 'Format Overview'!A19, 'Match Records Overview'!C:C, 'Format Overview'!C19)</f>
-        <v>0</v>
+      <c r="G19" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
       </c>
       <c r="H19">
         <f>SUMIFS('Match Records Overview'!J:J, 'Match Records Overview'!A:A, 'Format Overview'!A19, 'Match Records Overview'!C:C, 'Format Overview'!C19)</f>
@@ -3094,12 +4323,21 @@
         <f>SUMIFS('Match Records Overview'!K:K, 'Match Records Overview'!A:A, 'Format Overview'!A19, 'Match Records Overview'!C:C, 'Format Overview'!C19)</f>
         <v>0</v>
       </c>
+      <c r="J19">
+        <f>SUMIFS('Match Records Overview'!L:L, 'Match Records Overview'!A:A, 'Format Overview'!A19, 'Match Records Overview'!C:C, 'Format Overview'!C19)</f>
+        <v>0</v>
+      </c>
+      <c r="K19" s="12" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I19">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J19">
     <sortCondition ref="A2:A19"/>
     <sortCondition ref="C2:C19"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>